<commit_message>
Enable mapper 70 and AC-08 by default
</commit_message>
<xml_diff>
--- a/CoolGirl_rev6.x/board/bom.xlsx
+++ b/CoolGirl_rev6.x/board/bom.xlsx
@@ -309,15 +309,9 @@
     <t>SOT-223</t>
   </si>
   <si>
-    <t>C347229</t>
-  </si>
-  <si>
     <t>EPM1270T144C5N</t>
   </si>
   <si>
-    <t>LD1117-3.3</t>
-  </si>
-  <si>
     <t>LY62L2568LL-55LLI</t>
   </si>
   <si>
@@ -346,18 +340,32 @@
   </si>
   <si>
     <t>SOIC-28</t>
+  </si>
+  <si>
+    <t>C86781</t>
+  </si>
+  <si>
+    <t>LD1117S33TR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -439,17 +447,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -726,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1146,7 +1155,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>42</v>
@@ -1398,7 +1407,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>70</v>
@@ -1412,7 +1421,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>73</v>
@@ -1420,37 +1429,37 @@
       <c r="C49" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>86</v>
+      <c r="D49" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>74</v>
@@ -1464,7 +1473,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>77</v>
@@ -1478,7 +1487,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>80</v>
@@ -1492,7 +1501,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>81</v>
@@ -1506,7 +1515,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Changed flash to MT28EW01GABA1LJS
</commit_message>
<xml_diff>
--- a/CoolGirl_rev6.x/board/bom.xlsx
+++ b/CoolGirl_rev6.x/board/bom.xlsx
@@ -333,9 +333,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>S29GL01GP</t>
-  </si>
-  <si>
     <t>TSOP-56</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>LD1117S33TR</t>
+  </si>
+  <si>
+    <t>MT28EW01GABA1LJS</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>73</v>
@@ -1430,18 +1430,18 @@
         <v>85</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" s="4"/>
     </row>
@@ -1453,7 +1453,7 @@
         <v>92</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D51" s="4"/>
     </row>

</xml_diff>

<commit_message>
LY62L2568LL-55LLI replaced with LY62L2568RL-55LLI, center hole moved a bit, revision 6.3
</commit_message>
<xml_diff>
--- a/CoolGirl_rev6.x/board/bom.xlsx
+++ b/CoolGirl_rev6.x/board/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="92">
   <si>
     <t>Comment</t>
   </si>
@@ -276,12 +276,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>TSOP-32/8x14+20x0.5</t>
-  </si>
-  <si>
-    <t>C261875</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
@@ -306,82 +300,43 @@
     <t>U9</t>
   </si>
   <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>EPM1270T144C5N</t>
-  </si>
-  <si>
-    <t>LY62L2568LL-55LLI</t>
-  </si>
-  <si>
-    <t>74ALVC164245DGG:11</t>
-  </si>
-  <si>
-    <t>SN74LVC4245APWR</t>
-  </si>
-  <si>
-    <t>DIODE</t>
-  </si>
-  <si>
-    <t>FM18L08</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
     <t>U3</t>
   </si>
   <si>
-    <t>TSOP-56</t>
-  </si>
-  <si>
-    <t>SOIC-28</t>
-  </si>
-  <si>
-    <t>C86781</t>
-  </si>
-  <si>
-    <t>LD1117S33TR</t>
-  </si>
-  <si>
-    <t>MT28EW01GABA1LJS</t>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>SOT223-4</t>
+  </si>
+  <si>
+    <t>C347229</t>
+  </si>
+  <si>
+    <t>TSOP-56/14x20x0.5</t>
+  </si>
+  <si>
+    <t>SOIC-28/300mil</t>
+  </si>
+  <si>
+    <t>TSOP-32/8x14+20x0.5 b</t>
+  </si>
+  <si>
+    <t>C261876</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -447,20 +402,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -735,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1154,9 +1106,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
@@ -1406,9 +1356,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>70</v>
       </c>
@@ -1421,110 +1369,96 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>96</v>
+      <c r="C49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="3" t="s">
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="C54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="3" t="s">
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C56" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LD1117-3.3 replaced with LD1117S33TR
</commit_message>
<xml_diff>
--- a/CoolGirl_rev6.x/board/bom.xlsx
+++ b/CoolGirl_rev6.x/board/bom.xlsx
@@ -312,9 +312,6 @@
     <t>SOT223-4</t>
   </si>
   <si>
-    <t>C347229</t>
-  </si>
-  <si>
     <t>TSOP-56/14x20x0.5</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>C261876</t>
+  </si>
+  <si>
+    <t>C86781</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1378,7 +1378,7 @@
         <v>86</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1387,7 +1387,7 @@
         <v>84</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50" s="3"/>
     </row>
@@ -1397,7 +1397,7 @@
         <v>83</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="3"/>
     </row>
@@ -1407,10 +1407,10 @@
         <v>74</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:4">

</xml_diff>